<commit_message>
valida and invalid testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phani\eclipse-workspace\opencart\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09A5F9E-3023-4E9B-9E01-6D07B3BED89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D72BAD-6DB1-4AA8-B4BF-8F3DE93C9105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -388,22 +388,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F94931-CEC3-4EF9-A318-28F6ED4DDF78}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -413,11 +412,8 @@
       <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -427,11 +423,8 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -441,11 +434,8 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -455,11 +445,8 @@
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -469,11 +456,8 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -483,64 +467,12 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{ED226D99-CA7D-4A0B-805F-638D0151D7A2}"/>
-    <hyperlink ref="A4:A5" r:id="rId2" display="ethanhut@gmail.com" xr:uid="{53C5348C-E2EC-4643-A734-B2E9B13EE791}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{B72DF34A-C1DD-49B9-A21A-CA04052CEFBF}"/>
+    <hyperlink ref="A4:A5" r:id="rId2" display="ethanhut@gmail.com" xr:uid="{98FDBE2B-3455-474C-8D8D-9DB38F94C474}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>